<commit_message>
group-refactor2: numPersons, removed all 2 classes
</commit_message>
<xml_diff>
--- a/test/goa/india2.ffv.csv.xlsx
+++ b/test/goa/india2.ffv.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://broadridge-my.sharepoint.com/personal/john_nazareth_broadridge_com/Documents/personal/projects/gp/groupInXLS/test/goa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_D044345056948C2427400A4322EE6E96C9809867" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8031112-D993-41F5-A055-219F1DE0D7DB}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_D044345056948C2427400A4322EE6E96C9809867" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89B3CBD0-9B1F-4AE5-9E0E-436DB0B0DBD6}"/>
   <bookViews>
-    <workbookView xWindow="6564" yWindow="1032" windowWidth="15528" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5676" yWindow="708" windowWidth="15936" windowHeight="12144" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="moira.nazareth.inr.goa" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="185" r:id="rId3"/>
-    <pivotCache cacheId="189" r:id="rId4"/>
+    <pivotCache cacheId="35" r:id="rId3"/>
+    <pivotCache cacheId="39" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -415,7 +415,60 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Nazareth, John" refreshedDate="45404.423652430552" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="23" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Nazareth, John" refreshedDate="45438.573172453704" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A2:L4" sheet="moira.nazareth.usd.goa"/>
+  </cacheSource>
+  <cacheFields count="12">
+    <cacheField name="Item" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="1">
+        <s v="Hotel"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Vendor" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Description" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Amount" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="128.94" maxValue="237.29"/>
+    </cacheField>
+    <cacheField name="From" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="To" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Action" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="cn" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="42.98" maxValue="79.099999999999994"/>
+    </cacheField>
+    <cacheField name="gc" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="42.98" maxValue="79.099999999999994"/>
+    </cacheField>
+    <cacheField name="gd" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="jn" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="42.98" maxValue="79.099999999999994"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Nazareth, John" refreshedDate="45438.57317314815" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="23" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:L25" sheet="moira.nazareth.inr.goa"/>
   </cacheSource>
@@ -473,60 +526,40 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Nazareth, John" refreshedDate="45404.423652893522" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A2:L4" sheet="moira.nazareth.usd.goa"/>
-  </cacheSource>
-  <cacheFields count="12">
-    <cacheField name="Item" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Category" numFmtId="0">
-      <sharedItems count="1">
-        <s v="Hotel"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Vendor" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Description" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Amount" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="128.94" maxValue="237.29"/>
-    </cacheField>
-    <cacheField name="From" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="To" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Action" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="cn" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="42.98" maxValue="79.099999999999994"/>
-    </cacheField>
-    <cacheField name="gc" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="42.98" maxValue="79.099999999999994"/>
-    </cacheField>
-    <cacheField name="gd" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
-    </cacheField>
-    <cacheField name="jn" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="42.98" maxValue="79.099999999999994"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+  <r>
+    <s v="Tue 04.02"/>
+    <x v="0"/>
+    <s v=""/>
+    <s v="Agoda O'Pescador"/>
+    <n v="128.94"/>
+    <s v="jn"/>
+    <s v="jn, gc,cn"/>
+    <s v="jn (*:self), gd (*:self), gc (*:self), cn (*:self), moira.nazareth.usd.goa (*:group)"/>
+    <n v="42.98"/>
+    <n v="42.98"/>
+    <n v="0"/>
+    <n v="42.98"/>
+  </r>
+  <r>
+    <s v="Wed 04.03"/>
+    <x v="0"/>
+    <s v=""/>
+    <s v="Agoda StoneWood Hotel"/>
+    <n v="237.29"/>
+    <s v="jn"/>
+    <s v="jn, gc,cn"/>
+    <s v=""/>
+    <n v="79.099999999999994"/>
+    <n v="79.099999999999994"/>
+    <n v="0"/>
+    <n v="79.099999999999994"/>
+  </r>
+</pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="23">
   <r>
     <s v="Thu 03.28"/>
@@ -853,41 +886,8 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
-  <r>
-    <s v="Tue 04.02"/>
-    <x v="0"/>
-    <s v=""/>
-    <s v="Agoda O'Pescador"/>
-    <n v="128.94"/>
-    <s v="jn"/>
-    <s v="jn, gc,cn"/>
-    <s v="jn (*:self), gd (*:self), gc (*:self), cn (*:self), moira.nazareth.usd.goa (*:group)"/>
-    <n v="42.98"/>
-    <n v="42.98"/>
-    <n v="0"/>
-    <n v="42.98"/>
-  </r>
-  <r>
-    <s v="Wed 04.03"/>
-    <x v="0"/>
-    <s v=""/>
-    <s v="Agoda StoneWood Hotel"/>
-    <n v="237.29"/>
-    <s v="jn"/>
-    <s v="jn, gc,cn"/>
-    <s v=""/>
-    <n v="79.099999999999994"/>
-    <n v="79.099999999999994"/>
-    <n v="0"/>
-    <n v="79.099999999999994"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="185" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" multipleFieldFilters="0">
   <location ref="B27:F36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -976,7 +976,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable3" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable3" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" multipleFieldFilters="0">
   <location ref="B6:F9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -1041,9 +1041,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1081,7 +1081,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1187,7 +1187,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1329,7 +1329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3371,7 +3371,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>